<commit_message>
Array SD, Common SD, ConfigReader and config properties for stack
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Login.xlsx
+++ b/src/test/resources/Exceldata/Login.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -44,9 +44,6 @@
     <t>sdet86batch</t>
   </si>
   <si>
-    <t>dh2</t>
-  </si>
-  <si>
     <t>pythonCode</t>
   </si>
   <si>
@@ -57,13 +54,89 @@
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+print("Element Found")
+\b
+\b
+else:
+print("Not Found")
+\b
+\b
+\b
+\b
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>submission success</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+\b
+\b
+else:
+count+= 1
+\b
+\b
+result = max(result, count)
+\b
+\b
+print(result)
+\b
+\b
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+\b
+\b
+\b
+\b
+print c
+return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+\b
+\b
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -75,13 +148,23 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,12 +173,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -390,17 +479,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -418,29 +496,96 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="38.43"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified my pages Fri 3pm
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Login.xlsx
+++ b/src/test/resources/Exceldata/Login.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathy\work\SathyaWorkspace\dsAlgoProject\src\test\resources\Exceldata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D771D8-32FD-4140-B6D6-9D44097E80D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="pythonCode" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -131,24 +140,32 @@
   <si>
     <t>[4, 9, 9, 49, 121]</t>
   </si>
+  <si>
+    <t>Please check your user id</t>
+  </si>
+  <si>
+    <t>Please check your password</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -158,7 +175,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -168,43 +185,43 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -394,26 +411,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.43"/>
-    <col customWidth="1" min="2" max="2" width="11.71"/>
-    <col customWidth="1" min="3" max="3" width="28.14"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -432,10 +451,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,152 +462,140 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.43"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>